<commit_message>
ExcelDemo with market depth
</commit_message>
<xml_diff>
--- a/yats/config/ExcelDemo.xlsx
+++ b/yats/config/ExcelDemo.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiliano\IdeaProjects\AllGoTrading\yats\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="195" yWindow="135" windowWidth="13335" windowHeight="5805"/>
   </bookViews>
@@ -11,36 +16,196 @@
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Ask Px</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>ProductID</t>
   </si>
   <si>
-    <t>Bix Px</t>
-  </si>
-  <si>
     <t>OANDA_EURUSD</t>
   </si>
   <si>
-    <t>mid</t>
+    <t>Lv2 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv3 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv4 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv2 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv3 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv4 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv1 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv1 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv0 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv0 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv0 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv0 Ask Size</t>
+  </si>
+  <si>
+    <t>Lv1 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv1 Ask size</t>
+  </si>
+  <si>
+    <t>Lv2 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv2 Ask size</t>
+  </si>
+  <si>
+    <t>Lv3 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv3 Ask Size</t>
+  </si>
+  <si>
+    <t>Lv4 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv4 Ask Size</t>
+  </si>
+  <si>
+    <t>Lv5 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv5 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv5 Ask size</t>
+  </si>
+  <si>
+    <t>Lv5 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv6 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv6 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv6 Ask Size</t>
+  </si>
+  <si>
+    <t>Lv6 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv7 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv7 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv7 Ask Size</t>
+  </si>
+  <si>
+    <t>Lv7 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv8 Ask Px</t>
+  </si>
+  <si>
+    <t>Lv8 Ask Size</t>
+  </si>
+  <si>
+    <t>Lv8 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv8 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv9 Bid Size</t>
+  </si>
+  <si>
+    <t>Lv9 Bid Px</t>
+  </si>
+  <si>
+    <t>Lv9 Ask size</t>
+  </si>
+  <si>
+    <t>Lv9 Ask Px</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF339933"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,12 +231,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -80,9 +277,17 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF339933"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -131,7 +336,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,7 +371,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,58 +580,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:AO25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" customWidth="1"/>
+    <col min="23" max="25" width="11.5703125" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" customWidth="1"/>
+    <col min="27" max="27" width="11" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" customWidth="1"/>
+    <col min="30" max="30" width="10.7109375" customWidth="1"/>
+    <col min="31" max="31" width="12" customWidth="1"/>
+    <col min="32" max="32" width="10.28515625" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" customWidth="1"/>
+    <col min="34" max="34" width="10.42578125" customWidth="1"/>
+    <col min="35" max="35" width="10.140625" customWidth="1"/>
+    <col min="36" max="36" width="10.5703125" customWidth="1"/>
+    <col min="37" max="41" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1.34392</v>
-      </c>
-      <c r="C2">
-        <v>1.3441099999999999</v>
-      </c>
-      <c r="D2">
-        <f>(B2+C2)/2</f>
-        <v>1.344015</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="4">
+        <v>1.34114</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1.34124</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>